<commit_message>
DSGE - steady state and shocks
</commit_message>
<xml_diff>
--- a/Fiscal Consolidation and the Euro; the role of markups/data.xlsx
+++ b/Fiscal Consolidation and the Euro; the role of markups/data.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="101">
   <si>
     <t>x</t>
   </si>
@@ -75,6 +75,246 @@
   </si>
   <si>
     <t>20</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>31</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>34</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
+    <t>36</t>
+  </si>
+  <si>
+    <t>37</t>
+  </si>
+  <si>
+    <t>38</t>
+  </si>
+  <si>
+    <t>39</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>41</t>
+  </si>
+  <si>
+    <t>42</t>
+  </si>
+  <si>
+    <t>43</t>
+  </si>
+  <si>
+    <t>44</t>
+  </si>
+  <si>
+    <t>45</t>
+  </si>
+  <si>
+    <t>46</t>
+  </si>
+  <si>
+    <t>47</t>
+  </si>
+  <si>
+    <t>48</t>
+  </si>
+  <si>
+    <t>49</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>51</t>
+  </si>
+  <si>
+    <t>52</t>
+  </si>
+  <si>
+    <t>53</t>
+  </si>
+  <si>
+    <t>54</t>
+  </si>
+  <si>
+    <t>55</t>
+  </si>
+  <si>
+    <t>56</t>
+  </si>
+  <si>
+    <t>57</t>
+  </si>
+  <si>
+    <t>58</t>
+  </si>
+  <si>
+    <t>59</t>
+  </si>
+  <si>
+    <t>60</t>
+  </si>
+  <si>
+    <t>61</t>
+  </si>
+  <si>
+    <t>62</t>
+  </si>
+  <si>
+    <t>63</t>
+  </si>
+  <si>
+    <t>64</t>
+  </si>
+  <si>
+    <t>65</t>
+  </si>
+  <si>
+    <t>66</t>
+  </si>
+  <si>
+    <t>67</t>
+  </si>
+  <si>
+    <t>68</t>
+  </si>
+  <si>
+    <t>69</t>
+  </si>
+  <si>
+    <t>70</t>
+  </si>
+  <si>
+    <t>71</t>
+  </si>
+  <si>
+    <t>72</t>
+  </si>
+  <si>
+    <t>73</t>
+  </si>
+  <si>
+    <t>74</t>
+  </si>
+  <si>
+    <t>75</t>
+  </si>
+  <si>
+    <t>76</t>
+  </si>
+  <si>
+    <t>77</t>
+  </si>
+  <si>
+    <t>78</t>
+  </si>
+  <si>
+    <t>79</t>
+  </si>
+  <si>
+    <t>80</t>
+  </si>
+  <si>
+    <t>81</t>
+  </si>
+  <si>
+    <t>82</t>
+  </si>
+  <si>
+    <t>83</t>
+  </si>
+  <si>
+    <t>84</t>
+  </si>
+  <si>
+    <t>85</t>
+  </si>
+  <si>
+    <t>86</t>
+  </si>
+  <si>
+    <t>87</t>
+  </si>
+  <si>
+    <t>88</t>
+  </si>
+  <si>
+    <t>89</t>
+  </si>
+  <si>
+    <t>90</t>
+  </si>
+  <si>
+    <t>91</t>
+  </si>
+  <si>
+    <t>92</t>
+  </si>
+  <si>
+    <t>93</t>
+  </si>
+  <si>
+    <t>94</t>
+  </si>
+  <si>
+    <t>95</t>
+  </si>
+  <si>
+    <t>96</t>
+  </si>
+  <si>
+    <t>97</t>
+  </si>
+  <si>
+    <t>98</t>
+  </si>
+  <si>
+    <t>99</t>
+  </si>
+  <si>
+    <t>100</t>
   </si>
 </sst>
 </file>
@@ -136,7 +376,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>0.03155890425681385</v>
+        <v>0.042298723267627736</v>
       </c>
     </row>
     <row r="3">
@@ -144,7 +384,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>0.028636014520527553</v>
+        <v>0.055317456171751545</v>
       </c>
     </row>
     <row r="4">
@@ -152,7 +392,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>0.013261057821681632</v>
+        <v>0.018873099715422725</v>
       </c>
     </row>
     <row r="5">
@@ -160,7 +400,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>0.0024041760926838407</v>
+        <v>0.0020665418535603663</v>
       </c>
     </row>
     <row r="6">
@@ -168,7 +408,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>-0.00802565688167256</v>
+        <v>-0.02996877620465277</v>
       </c>
     </row>
     <row r="7">
@@ -176,7 +416,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>-0.007496273548877497</v>
+        <v>-0.08271935257304719</v>
       </c>
     </row>
     <row r="8">
@@ -184,7 +424,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>-0.02448979932725237</v>
+        <v>-0.08007936597462084</v>
       </c>
     </row>
     <row r="9">
@@ -192,7 +432,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>-0.035572526830859985</v>
+        <v>-0.12112211609199619</v>
       </c>
     </row>
     <row r="10">
@@ -200,7 +440,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>-0.04394775703541143</v>
+        <v>-0.13533540672962374</v>
       </c>
     </row>
     <row r="11">
@@ -208,7 +448,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>-0.046406517424941285</v>
+        <v>-0.14076120635316158</v>
       </c>
     </row>
     <row r="12">
@@ -216,7 +456,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>-0.05749831844242159</v>
+        <v>-0.15686057820866317</v>
       </c>
     </row>
     <row r="13">
@@ -224,7 +464,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>-0.06287822590563685</v>
+        <v>-0.14212639729017518</v>
       </c>
     </row>
     <row r="14">
@@ -232,7 +472,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>-0.06715282340150708</v>
+        <v>-0.14034305514963208</v>
       </c>
     </row>
     <row r="15">
@@ -240,7 +480,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>-0.07042520873613256</v>
+        <v>-0.12256552560047496</v>
       </c>
     </row>
     <row r="16">
@@ -248,7 +488,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="n">
-        <v>-0.07611812558725362</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="17">
@@ -256,7 +496,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="n">
-        <v>-0.06144956530319412</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="18">
@@ -264,7 +504,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="n">
-        <v>-0.06592783983510309</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="19">
@@ -272,7 +512,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="n">
-        <v>-0.06770952352158055</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="20">
@@ -280,7 +520,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="n">
-        <v>-0.06907833195330326</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="21">
@@ -288,7 +528,647 @@
         <v>20</v>
       </c>
       <c r="B21" t="n">
-        <v>-0.06641413007845998</v>
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>25</v>
+      </c>
+      <c r="B26" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>27</v>
+      </c>
+      <c r="B28" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>29</v>
+      </c>
+      <c r="B30" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>30</v>
+      </c>
+      <c r="B31" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>31</v>
+      </c>
+      <c r="B32" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B33" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s">
+        <v>33</v>
+      </c>
+      <c r="B34" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s">
+        <v>34</v>
+      </c>
+      <c r="B35" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s">
+        <v>35</v>
+      </c>
+      <c r="B36" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s">
+        <v>36</v>
+      </c>
+      <c r="B37" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s">
+        <v>37</v>
+      </c>
+      <c r="B38" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s">
+        <v>38</v>
+      </c>
+      <c r="B39" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s">
+        <v>39</v>
+      </c>
+      <c r="B40" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s">
+        <v>40</v>
+      </c>
+      <c r="B41" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s">
+        <v>41</v>
+      </c>
+      <c r="B42" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s">
+        <v>42</v>
+      </c>
+      <c r="B43" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s">
+        <v>43</v>
+      </c>
+      <c r="B44" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s">
+        <v>44</v>
+      </c>
+      <c r="B45" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s">
+        <v>45</v>
+      </c>
+      <c r="B46" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s">
+        <v>46</v>
+      </c>
+      <c r="B47" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s">
+        <v>47</v>
+      </c>
+      <c r="B48" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s">
+        <v>48</v>
+      </c>
+      <c r="B49" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s">
+        <v>49</v>
+      </c>
+      <c r="B50" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="s">
+        <v>50</v>
+      </c>
+      <c r="B51" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="s">
+        <v>51</v>
+      </c>
+      <c r="B52" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="s">
+        <v>52</v>
+      </c>
+      <c r="B53" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s">
+        <v>53</v>
+      </c>
+      <c r="B54" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="s">
+        <v>54</v>
+      </c>
+      <c r="B55" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="s">
+        <v>55</v>
+      </c>
+      <c r="B56" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="s">
+        <v>56</v>
+      </c>
+      <c r="B57" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="s">
+        <v>57</v>
+      </c>
+      <c r="B58" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="s">
+        <v>58</v>
+      </c>
+      <c r="B59" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="s">
+        <v>59</v>
+      </c>
+      <c r="B60" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="s">
+        <v>60</v>
+      </c>
+      <c r="B61" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="s">
+        <v>61</v>
+      </c>
+      <c r="B62" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="s">
+        <v>62</v>
+      </c>
+      <c r="B63" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="s">
+        <v>63</v>
+      </c>
+      <c r="B64" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="s">
+        <v>64</v>
+      </c>
+      <c r="B65" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="s">
+        <v>65</v>
+      </c>
+      <c r="B66" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="s">
+        <v>66</v>
+      </c>
+      <c r="B67" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="s">
+        <v>67</v>
+      </c>
+      <c r="B68" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="s">
+        <v>68</v>
+      </c>
+      <c r="B69" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="s">
+        <v>69</v>
+      </c>
+      <c r="B70" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="s">
+        <v>70</v>
+      </c>
+      <c r="B71" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="s">
+        <v>71</v>
+      </c>
+      <c r="B72" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="s">
+        <v>72</v>
+      </c>
+      <c r="B73" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="s">
+        <v>73</v>
+      </c>
+      <c r="B74" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="s">
+        <v>74</v>
+      </c>
+      <c r="B75" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="s">
+        <v>75</v>
+      </c>
+      <c r="B76" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="s">
+        <v>76</v>
+      </c>
+      <c r="B77" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="s">
+        <v>77</v>
+      </c>
+      <c r="B78" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="s">
+        <v>78</v>
+      </c>
+      <c r="B79" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="s">
+        <v>79</v>
+      </c>
+      <c r="B80" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="s">
+        <v>80</v>
+      </c>
+      <c r="B81" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="s">
+        <v>81</v>
+      </c>
+      <c r="B82" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="s">
+        <v>82</v>
+      </c>
+      <c r="B83" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="s">
+        <v>83</v>
+      </c>
+      <c r="B84" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="s">
+        <v>84</v>
+      </c>
+      <c r="B85" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="s">
+        <v>85</v>
+      </c>
+      <c r="B86" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="s">
+        <v>86</v>
+      </c>
+      <c r="B87" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="s">
+        <v>87</v>
+      </c>
+      <c r="B88" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="s">
+        <v>88</v>
+      </c>
+      <c r="B89" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="s">
+        <v>89</v>
+      </c>
+      <c r="B90" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="s">
+        <v>90</v>
+      </c>
+      <c r="B91" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="s">
+        <v>91</v>
+      </c>
+      <c r="B92" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="s">
+        <v>92</v>
+      </c>
+      <c r="B93" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="s">
+        <v>93</v>
+      </c>
+      <c r="B94" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="s">
+        <v>94</v>
+      </c>
+      <c r="B95" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="s">
+        <v>95</v>
+      </c>
+      <c r="B96" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="s">
+        <v>96</v>
+      </c>
+      <c r="B97" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="s">
+        <v>97</v>
+      </c>
+      <c r="B98" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="s">
+        <v>98</v>
+      </c>
+      <c r="B99" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="s">
+        <v>99</v>
+      </c>
+      <c r="B100" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="s">
+        <v>100</v>
+      </c>
+      <c r="B101" t="n">
+        <v>0.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>